<commit_message>
This 14 march 1 sit commit
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/LoginData.xlsx
+++ b/src/test/java/TestData/LoginData.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -23,7 +22,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>locked_out_user</t>
+    <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
@@ -32,16 +31,7 @@
     <t>problem_user</t>
   </si>
   <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
     <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>standard_user</t>
   </si>
 </sst>
 </file>
@@ -663,12 +653,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,80 +1002,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="25.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="13.4285714285714" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1107,7 +1024,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1115,7 +1032,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1123,7 +1040,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>